<commit_message>
bento: KMR005: update file template
</commit_message>
<xml_diff>
--- a/nts.uk/uk.at/at.file/nts.uk.file.at.infra/src/main/resources/report/帳票イメージ-KMR005_月間予約台帳.xlsx
+++ b/nts.uk/uk.at/at.file/nts.uk.file.at.infra/src/main/resources/report/帳票イメージ-KMR005_月間予約台帳.xlsx
@@ -9,10 +9,10 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3810" yWindow="-120" windowWidth="28005" windowHeight="16440"/>
+    <workbookView xWindow="4740" yWindow="-120" windowWidth="28005" windowHeight="16440"/>
   </bookViews>
   <sheets>
-    <sheet name="月間予約台帳" sheetId="9" r:id="rId1"/>
+    <sheet name="月間予約台帳" sheetId="11" r:id="rId1"/>
   </sheets>
   <externalReferences>
     <externalReference r:id="rId2"/>
@@ -238,7 +238,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="14">
   <si>
     <t>社員</t>
     <rPh sb="0" eb="2">
@@ -254,23 +254,16 @@
     <phoneticPr fontId="3"/>
   </si>
   <si>
-    <t>合計</t>
+    <t>単価</t>
     <rPh sb="0" eb="2">
-      <t>ゴウケイ</t>
+      <t>タンカ</t>
     </rPh>
     <phoneticPr fontId="3"/>
   </si>
   <si>
-    <t>商品１</t>
-    <rPh sb="0" eb="1">
-      <t>ショウヒン</t>
-    </rPh>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>商品２</t>
-    <rPh sb="0" eb="1">
-      <t>ショウヒン</t>
+    <t>合計</t>
+    <rPh sb="0" eb="2">
+      <t>ゴウケイ</t>
     </rPh>
     <phoneticPr fontId="3"/>
   </si>
@@ -309,43 +302,16 @@
     <phoneticPr fontId="3"/>
   </si>
   <si>
-    <t>金</t>
-    <rPh sb="0" eb="1">
-      <t>キン</t>
+    <t>補助金</t>
+    <rPh sb="0" eb="3">
+      <t>ホジョキン</t>
     </rPh>
     <phoneticPr fontId="3"/>
   </si>
   <si>
-    <t>0010000001 開発本部</t>
-    <rPh sb="11" eb="13">
-      <t>カイハツ</t>
-    </rPh>
-    <rPh sb="13" eb="15">
-      <t>ホンブ</t>
-    </rPh>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>00000001 日通 太郎</t>
-    <rPh sb="9" eb="11">
-      <t>ニッツウ</t>
-    </rPh>
-    <rPh sb="12" eb="14">
-      <t>タロウ</t>
-    </rPh>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>金額2</t>
-    <rPh sb="0" eb="2">
-      <t>キンガク</t>
-    </rPh>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>金額1</t>
-    <rPh sb="0" eb="2">
-      <t>キンガク</t>
+    <t>金</t>
+    <rPh sb="0" eb="1">
+      <t>キン</t>
     </rPh>
     <phoneticPr fontId="3"/>
   </si>
@@ -416,7 +382,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="21">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -627,11 +593,13 @@
       <left style="dotted">
         <color indexed="64"/>
       </left>
-      <right/>
-      <top style="double">
+      <right style="dotted">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
+      <bottom style="double">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -639,23 +607,10 @@
     <border>
       <left/>
       <right/>
-      <top style="double">
+      <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="dotted">
-        <color indexed="64"/>
-      </right>
-      <top style="double">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
+      <bottom style="double">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -669,7 +624,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -700,17 +655,14 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="14" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="38" fontId="2" fillId="2" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="38" fontId="2" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
@@ -721,22 +673,13 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="38" fontId="2" fillId="2" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="38" fontId="2" fillId="5" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="38" fontId="2" fillId="5" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -821,7 +764,7 @@
       <sheetName val="master"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="0"/>
       <sheetData sheetId="1" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
@@ -845,17 +788,17 @@
       <sheetName val="内示書"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
-      <sheetData sheetId="6" refreshError="1"/>
-      <sheetData sheetId="7" refreshError="1"/>
-      <sheetData sheetId="8" refreshError="1"/>
-      <sheetData sheetId="9" refreshError="1"/>
-      <sheetData sheetId="10" refreshError="1"/>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -2351,10 +2294,10 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
       <sheetData sheetId="5" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
@@ -44394,8 +44337,8 @@
   </sheetPr>
   <dimension ref="B1:AK12"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageLayout" zoomScale="70" zoomScaleNormal="130" zoomScaleSheetLayoutView="115" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="BS2" sqref="BS2"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageLayout" zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="115" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.140625" defaultRowHeight="11.25"/>
@@ -44413,7 +44356,7 @@
   <sheetData>
     <row r="1" spans="2:37" ht="12" thickBot="1">
       <c r="B1" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
@@ -44452,10 +44395,10 @@
       <c r="AK1" s="4"/>
     </row>
     <row r="2" spans="2:37" ht="9.75" customHeight="1">
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="28" t="s">
+      <c r="C2" s="24" t="s">
         <v>1</v>
       </c>
       <c r="D2" s="5">
@@ -44551,166 +44494,158 @@
       <c r="AH2" s="5">
         <v>31</v>
       </c>
-      <c r="AI2" s="30" t="s">
+      <c r="AI2" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="AJ2" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="AJ2" s="30" t="s">
-        <v>17</v>
-      </c>
-      <c r="AK2" s="32" t="s">
-        <v>16</v>
+      <c r="AK2" s="28" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="2:37" ht="9.75" customHeight="1" thickBot="1">
-      <c r="B3" s="27"/>
-      <c r="C3" s="29"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="25"/>
       <c r="D3" s="6" t="s">
         <v>13</v>
       </c>
       <c r="E3" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="G3" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="H3" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="H3" s="6" t="s">
-        <v>11</v>
+      <c r="I3" s="6" t="s">
+        <v>4</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="J3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="J3" s="6" t="s">
+      <c r="K3" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="K3" s="6" t="s">
+      <c r="L3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="L3" s="6" t="s">
+      <c r="M3" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="M3" s="6" t="s">
+      <c r="N3" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="N3" s="6" t="s">
+      <c r="O3" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="O3" s="6" t="s">
-        <v>11</v>
+      <c r="P3" s="6" t="s">
+        <v>4</v>
       </c>
-      <c r="P3" s="6" t="s">
+      <c r="Q3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="Q3" s="6" t="s">
+      <c r="R3" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="R3" s="6" t="s">
+      <c r="S3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="S3" s="6" t="s">
+      <c r="T3" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="T3" s="6" t="s">
+      <c r="U3" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="U3" s="6" t="s">
+      <c r="V3" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="V3" s="6" t="s">
-        <v>11</v>
+      <c r="W3" s="6" t="s">
+        <v>4</v>
       </c>
-      <c r="W3" s="6" t="s">
+      <c r="X3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="X3" s="6" t="s">
+      <c r="Y3" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="Y3" s="6" t="s">
+      <c r="Z3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="Z3" s="6" t="s">
+      <c r="AA3" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="AA3" s="6" t="s">
+      <c r="AB3" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="AB3" s="6" t="s">
+      <c r="AC3" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="AC3" s="6" t="s">
-        <v>11</v>
+      <c r="AD3" s="6" t="s">
+        <v>4</v>
       </c>
-      <c r="AD3" s="6" t="s">
+      <c r="AE3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="AE3" s="6" t="s">
+      <c r="AF3" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="AF3" s="6" t="s">
+      <c r="AG3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="AG3" s="6" t="s">
+      <c r="AH3" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="AH3" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="AI3" s="31"/>
-      <c r="AJ3" s="31"/>
-      <c r="AK3" s="33"/>
+      <c r="AI3" s="27"/>
+      <c r="AJ3" s="27"/>
+      <c r="AK3" s="29"/>
     </row>
     <row r="4" spans="2:37" ht="9.75" customHeight="1">
-      <c r="B4" s="34" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="35"/>
-      <c r="D4" s="35"/>
-      <c r="E4" s="35"/>
-      <c r="F4" s="35"/>
-      <c r="G4" s="35"/>
-      <c r="H4" s="35"/>
-      <c r="I4" s="35"/>
-      <c r="J4" s="35"/>
-      <c r="K4" s="35"/>
-      <c r="L4" s="35"/>
-      <c r="M4" s="35"/>
-      <c r="N4" s="35"/>
-      <c r="O4" s="35"/>
-      <c r="P4" s="35"/>
-      <c r="Q4" s="35"/>
-      <c r="R4" s="35"/>
-      <c r="S4" s="35"/>
-      <c r="T4" s="35"/>
-      <c r="U4" s="35"/>
-      <c r="V4" s="35"/>
-      <c r="W4" s="35"/>
-      <c r="X4" s="35"/>
-      <c r="Y4" s="35"/>
-      <c r="Z4" s="35"/>
-      <c r="AA4" s="35"/>
-      <c r="AB4" s="35"/>
-      <c r="AC4" s="35"/>
-      <c r="AD4" s="35"/>
-      <c r="AE4" s="35"/>
-      <c r="AF4" s="35"/>
-      <c r="AG4" s="35"/>
-      <c r="AH4" s="35"/>
-      <c r="AI4" s="35"/>
-      <c r="AJ4" s="35"/>
-      <c r="AK4" s="36"/>
+      <c r="B4" s="30"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="31"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="31"/>
+      <c r="I4" s="31"/>
+      <c r="J4" s="31"/>
+      <c r="K4" s="31"/>
+      <c r="L4" s="31"/>
+      <c r="M4" s="31"/>
+      <c r="N4" s="31"/>
+      <c r="O4" s="31"/>
+      <c r="P4" s="31"/>
+      <c r="Q4" s="31"/>
+      <c r="R4" s="31"/>
+      <c r="S4" s="31"/>
+      <c r="T4" s="31"/>
+      <c r="U4" s="31"/>
+      <c r="V4" s="31"/>
+      <c r="W4" s="31"/>
+      <c r="X4" s="31"/>
+      <c r="Y4" s="31"/>
+      <c r="Z4" s="31"/>
+      <c r="AA4" s="31"/>
+      <c r="AB4" s="31"/>
+      <c r="AC4" s="31"/>
+      <c r="AD4" s="31"/>
+      <c r="AE4" s="31"/>
+      <c r="AF4" s="31"/>
+      <c r="AG4" s="31"/>
+      <c r="AH4" s="31"/>
+      <c r="AI4" s="31"/>
+      <c r="AJ4" s="31"/>
+      <c r="AK4" s="32"/>
     </row>
     <row r="5" spans="2:37" ht="9.75" customHeight="1">
-      <c r="B5" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="D5" s="8">
-        <v>1</v>
-      </c>
+      <c r="B5" s="19"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="8"/>
       <c r="E5" s="8"/>
       <c r="F5" s="8"/>
       <c r="G5" s="8"/>
@@ -44723,9 +44658,7 @@
       <c r="N5" s="8"/>
       <c r="O5" s="8"/>
       <c r="P5" s="8"/>
-      <c r="Q5" s="8">
-        <v>1</v>
-      </c>
+      <c r="Q5" s="8"/>
       <c r="R5" s="8"/>
       <c r="S5" s="8"/>
       <c r="T5" s="8"/>
@@ -44738,130 +44671,93 @@
       <c r="AA5" s="9"/>
       <c r="AB5" s="9"/>
       <c r="AC5" s="9"/>
-      <c r="AD5" s="9">
-        <v>1</v>
-      </c>
+      <c r="AD5" s="9"/>
       <c r="AE5" s="9"/>
       <c r="AF5" s="9"/>
       <c r="AG5" s="9"/>
       <c r="AH5" s="9"/>
-      <c r="AI5" s="9">
-        <f>SUM(D5:AH5)</f>
-        <v>3</v>
-      </c>
-      <c r="AJ5" s="17">
-        <f>AL$5*AI5</f>
-        <v>0</v>
-      </c>
-      <c r="AK5" s="17">
-        <f>AM$5*AI5</f>
-        <v>0</v>
-      </c>
+      <c r="AI5" s="9"/>
+      <c r="AJ5" s="10"/>
+      <c r="AK5" s="11"/>
     </row>
     <row r="6" spans="2:37" ht="9.75" customHeight="1" thickBot="1">
-      <c r="B6" s="24"/>
-      <c r="C6" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11">
-        <v>1</v>
-      </c>
-      <c r="H6" s="11"/>
-      <c r="I6" s="11"/>
-      <c r="J6" s="11"/>
-      <c r="K6" s="11"/>
-      <c r="L6" s="11"/>
-      <c r="M6" s="11"/>
-      <c r="N6" s="11"/>
-      <c r="O6" s="11"/>
-      <c r="P6" s="11"/>
-      <c r="Q6" s="11"/>
-      <c r="R6" s="11">
-        <v>1</v>
-      </c>
-      <c r="S6" s="11"/>
-      <c r="T6" s="11"/>
-      <c r="U6" s="11"/>
-      <c r="V6" s="11"/>
-      <c r="W6" s="12"/>
-      <c r="X6" s="12"/>
-      <c r="Y6" s="12"/>
-      <c r="Z6" s="12"/>
-      <c r="AA6" s="12"/>
-      <c r="AB6" s="12"/>
-      <c r="AC6" s="12"/>
-      <c r="AD6" s="12"/>
-      <c r="AE6" s="12">
-        <v>1</v>
-      </c>
-      <c r="AF6" s="12"/>
-      <c r="AG6" s="12"/>
-      <c r="AH6" s="12"/>
-      <c r="AI6" s="12">
-        <f t="shared" ref="AI6" si="0">SUM(D6:AH6)</f>
-        <v>3</v>
-      </c>
-      <c r="AJ6" s="18">
-        <f>AL$6*AI6</f>
-        <v>0</v>
-      </c>
-      <c r="AK6" s="19">
-        <f>AM$6*AI6</f>
-        <v>0</v>
-      </c>
+      <c r="B6" s="20"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="16"/>
+      <c r="I6" s="16"/>
+      <c r="J6" s="16"/>
+      <c r="K6" s="16"/>
+      <c r="L6" s="16"/>
+      <c r="M6" s="16"/>
+      <c r="N6" s="16"/>
+      <c r="O6" s="16"/>
+      <c r="P6" s="16"/>
+      <c r="Q6" s="16"/>
+      <c r="R6" s="16"/>
+      <c r="S6" s="16"/>
+      <c r="T6" s="16"/>
+      <c r="U6" s="16"/>
+      <c r="V6" s="16"/>
+      <c r="W6" s="17"/>
+      <c r="X6" s="17"/>
+      <c r="Y6" s="17"/>
+      <c r="Z6" s="17"/>
+      <c r="AA6" s="17"/>
+      <c r="AB6" s="17"/>
+      <c r="AC6" s="17"/>
+      <c r="AD6" s="17"/>
+      <c r="AE6" s="17"/>
+      <c r="AF6" s="17"/>
+      <c r="AG6" s="17"/>
+      <c r="AH6" s="17"/>
+      <c r="AI6" s="17"/>
+      <c r="AJ6" s="17"/>
+      <c r="AK6" s="18"/>
     </row>
     <row r="7" spans="2:37" ht="9.75" customHeight="1" thickTop="1">
-      <c r="B7" s="25"/>
-      <c r="C7" s="20"/>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="21"/>
-      <c r="G7" s="21"/>
-      <c r="H7" s="21"/>
-      <c r="I7" s="21"/>
-      <c r="J7" s="21"/>
-      <c r="K7" s="21"/>
-      <c r="L7" s="21"/>
-      <c r="M7" s="21"/>
-      <c r="N7" s="21"/>
-      <c r="O7" s="21"/>
-      <c r="P7" s="21"/>
-      <c r="Q7" s="21"/>
-      <c r="R7" s="21"/>
-      <c r="S7" s="21"/>
-      <c r="T7" s="21"/>
-      <c r="U7" s="21"/>
-      <c r="V7" s="21"/>
-      <c r="W7" s="21"/>
-      <c r="X7" s="21"/>
-      <c r="Y7" s="21"/>
-      <c r="Z7" s="21"/>
-      <c r="AA7" s="21"/>
-      <c r="AB7" s="21"/>
-      <c r="AC7" s="21"/>
-      <c r="AD7" s="21"/>
-      <c r="AE7" s="21"/>
-      <c r="AF7" s="21"/>
-      <c r="AG7" s="21"/>
-      <c r="AH7" s="22"/>
-      <c r="AI7" s="13">
-        <f>SUM(AI5:AI6)</f>
-        <v>6</v>
-      </c>
-      <c r="AJ7" s="14">
-        <f>SUM(AJ5:AJ6)</f>
-        <v>0</v>
-      </c>
-      <c r="AK7" s="15">
-        <f>SUM(AK5:AK6)</f>
-        <v>0</v>
-      </c>
+      <c r="B7" s="21"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="13"/>
+      <c r="J7" s="13"/>
+      <c r="K7" s="13"/>
+      <c r="L7" s="13"/>
+      <c r="M7" s="13"/>
+      <c r="N7" s="13"/>
+      <c r="O7" s="13"/>
+      <c r="P7" s="13"/>
+      <c r="Q7" s="13"/>
+      <c r="R7" s="13"/>
+      <c r="S7" s="13"/>
+      <c r="T7" s="13"/>
+      <c r="U7" s="13"/>
+      <c r="V7" s="13"/>
+      <c r="W7" s="13"/>
+      <c r="X7" s="13"/>
+      <c r="Y7" s="13"/>
+      <c r="Z7" s="13"/>
+      <c r="AA7" s="13"/>
+      <c r="AB7" s="13"/>
+      <c r="AC7" s="13"/>
+      <c r="AD7" s="13"/>
+      <c r="AE7" s="13"/>
+      <c r="AF7" s="13"/>
+      <c r="AG7" s="13"/>
+      <c r="AH7" s="13"/>
+      <c r="AI7" s="13"/>
+      <c r="AJ7" s="13"/>
+      <c r="AK7" s="14"/>
     </row>
     <row r="8" spans="2:37" ht="9.75" customHeight="1">
-      <c r="C8" s="16"/>
+      <c r="C8" s="15"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
@@ -44898,7 +44794,7 @@
       <c r="AK8" s="3"/>
     </row>
     <row r="9" spans="2:37" ht="9.75" customHeight="1">
-      <c r="C9" s="16"/>
+      <c r="C9" s="15"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
@@ -44973,13 +44869,13 @@
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="AJ2:AJ3"/>
+    <mergeCell ref="AK2:AK3"/>
+    <mergeCell ref="B4:AK4"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="C2:C3"/>
     <mergeCell ref="AI2:AI3"/>
-    <mergeCell ref="AJ2:AJ3"/>
-    <mergeCell ref="AK2:AK3"/>
-    <mergeCell ref="B4:AK4"/>
   </mergeCells>
   <phoneticPr fontId="3"/>
   <printOptions horizontalCentered="1"/>
@@ -44987,7 +44883,7 @@
   <pageSetup paperSize="9" scale="99" orientation="landscape" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;L&amp;"MSゴシック,標準"日通システム株式会社
-&amp;C&amp;"MSゴシック,太字"&amp;16月間予約台帳&amp;R&amp;"MSゴシック,標準"&amp;D　&amp;T　
+&amp;C&amp;"MSゴシック,太字"&amp;16月間予約&amp;R&amp;"MSゴシック,標準"&amp;D　&amp;T　
 page&amp;P</oddHeader>
   </headerFooter>
   <rowBreaks count="1" manualBreakCount="1">

</xml_diff>

<commit_message>
bento: KMR005: sửa lỗi border double
</commit_message>
<xml_diff>
--- a/nts.uk/uk.at/at.file/nts.uk.file.at.infra/src/main/resources/report/帳票イメージ-KMR005_月間予約台帳.xlsx
+++ b/nts.uk/uk.at/at.file/nts.uk.file.at.infra/src/main/resources/report/帳票イメージ-KMR005_月間予約台帳.xlsx
@@ -12,7 +12,7 @@
     <workbookView xWindow="4740" yWindow="-120" windowWidth="28005" windowHeight="16440"/>
   </bookViews>
   <sheets>
-    <sheet name="月間予約台帳" sheetId="11" r:id="rId1"/>
+    <sheet name="月間予約台帳" sheetId="9" r:id="rId1"/>
   </sheets>
   <externalReferences>
     <externalReference r:id="rId2"/>
@@ -238,28 +238,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="14">
-  <si>
-    <t>社員</t>
-    <rPh sb="0" eb="2">
-      <t>シャイン</t>
-    </rPh>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>名称</t>
-    <rPh sb="0" eb="2">
-      <t>メイショウ</t>
-    </rPh>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>単価</t>
-    <rPh sb="0" eb="2">
-      <t>タンカ</t>
-    </rPh>
-    <phoneticPr fontId="3"/>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="12">
   <si>
     <t>合計</t>
     <rPh sb="0" eb="2">
@@ -302,16 +281,23 @@
     <phoneticPr fontId="3"/>
   </si>
   <si>
-    <t>補助金</t>
-    <rPh sb="0" eb="3">
-      <t>ホジョキン</t>
+    <t>金</t>
+    <rPh sb="0" eb="1">
+      <t>キン</t>
     </rPh>
     <phoneticPr fontId="3"/>
   </si>
   <si>
-    <t>金</t>
-    <rPh sb="0" eb="1">
-      <t>キン</t>
+    <t>金額2</t>
+    <rPh sb="0" eb="2">
+      <t>キンガク</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>金額1</t>
+    <rPh sb="0" eb="2">
+      <t>キンガク</t>
     </rPh>
     <phoneticPr fontId="3"/>
   </si>
@@ -382,7 +368,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="20">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -593,13 +579,11 @@
       <left style="dotted">
         <color indexed="64"/>
       </left>
-      <right style="dotted">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
+      <right/>
+      <top style="double">
         <color indexed="64"/>
       </top>
-      <bottom style="double">
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -607,10 +591,23 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
+      <top style="double">
         <color indexed="64"/>
       </top>
-      <bottom style="double">
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="dotted">
+        <color indexed="64"/>
+      </right>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -624,7 +621,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -655,14 +652,17 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="38" fontId="2" fillId="2" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="14" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="38" fontId="2" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
@@ -673,13 +673,22 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="38" fontId="2" fillId="2" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="38" fontId="2" fillId="5" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="38" fontId="2" fillId="5" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -44337,8 +44346,8 @@
   </sheetPr>
   <dimension ref="B1:AK12"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageLayout" zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="115" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageLayout" zoomScale="115" zoomScaleNormal="130" zoomScaleSheetLayoutView="115" zoomScalePageLayoutView="115" workbookViewId="0">
+      <selection activeCell="AC6" sqref="AC6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.140625" defaultRowHeight="11.25"/>
@@ -44356,7 +44365,7 @@
   <sheetData>
     <row r="1" spans="2:37" ht="12" thickBot="1">
       <c r="B1" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
@@ -44395,12 +44404,8 @@
       <c r="AK1" s="4"/>
     </row>
     <row r="2" spans="2:37" ht="9.75" customHeight="1">
-      <c r="B2" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="24" t="s">
-        <v>1</v>
-      </c>
+      <c r="B2" s="26"/>
+      <c r="C2" s="28"/>
       <c r="D2" s="5">
         <v>1</v>
       </c>
@@ -44494,156 +44499,156 @@
       <c r="AH2" s="5">
         <v>31</v>
       </c>
-      <c r="AI2" s="26" t="s">
-        <v>3</v>
+      <c r="AI2" s="30" t="s">
+        <v>0</v>
       </c>
-      <c r="AJ2" s="26" t="s">
-        <v>2</v>
+      <c r="AJ2" s="30" t="s">
+        <v>11</v>
       </c>
-      <c r="AK2" s="28" t="s">
-        <v>12</v>
+      <c r="AK2" s="32" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="2:37" ht="9.75" customHeight="1" thickBot="1">
-      <c r="B3" s="23"/>
-      <c r="C3" s="25"/>
+      <c r="B3" s="27"/>
+      <c r="C3" s="29"/>
       <c r="D3" s="6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E3" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="6" t="s">
-        <v>8</v>
+      <c r="I3" s="6" t="s">
+        <v>1</v>
       </c>
-      <c r="G3" s="6" t="s">
-        <v>9</v>
+      <c r="J3" s="6" t="s">
+        <v>2</v>
       </c>
-      <c r="H3" s="6" t="s">
-        <v>10</v>
+      <c r="K3" s="6" t="s">
+        <v>3</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="L3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="J3" s="6" t="s">
+      <c r="M3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="K3" s="6" t="s">
+      <c r="N3" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="L3" s="6" t="s">
+      <c r="O3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="M3" s="6" t="s">
-        <v>8</v>
+      <c r="P3" s="6" t="s">
+        <v>1</v>
       </c>
-      <c r="N3" s="6" t="s">
-        <v>9</v>
+      <c r="Q3" s="6" t="s">
+        <v>2</v>
       </c>
-      <c r="O3" s="6" t="s">
-        <v>10</v>
+      <c r="R3" s="6" t="s">
+        <v>3</v>
       </c>
-      <c r="P3" s="6" t="s">
+      <c r="S3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="Q3" s="6" t="s">
+      <c r="T3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="R3" s="6" t="s">
+      <c r="U3" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="S3" s="6" t="s">
+      <c r="V3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="T3" s="6" t="s">
-        <v>8</v>
+      <c r="W3" s="6" t="s">
+        <v>1</v>
       </c>
-      <c r="U3" s="6" t="s">
-        <v>9</v>
+      <c r="X3" s="6" t="s">
+        <v>2</v>
       </c>
-      <c r="V3" s="6" t="s">
-        <v>10</v>
+      <c r="Y3" s="6" t="s">
+        <v>3</v>
       </c>
-      <c r="W3" s="6" t="s">
+      <c r="Z3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="X3" s="6" t="s">
+      <c r="AA3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="Y3" s="6" t="s">
+      <c r="AB3" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="Z3" s="6" t="s">
+      <c r="AC3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="AA3" s="6" t="s">
-        <v>8</v>
+      <c r="AD3" s="6" t="s">
+        <v>1</v>
       </c>
-      <c r="AB3" s="6" t="s">
-        <v>9</v>
+      <c r="AE3" s="6" t="s">
+        <v>2</v>
       </c>
-      <c r="AC3" s="6" t="s">
-        <v>10</v>
+      <c r="AF3" s="6" t="s">
+        <v>3</v>
       </c>
-      <c r="AD3" s="6" t="s">
+      <c r="AG3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="AE3" s="6" t="s">
+      <c r="AH3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="AF3" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="AG3" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="AH3" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="AI3" s="27"/>
-      <c r="AJ3" s="27"/>
-      <c r="AK3" s="29"/>
+      <c r="AI3" s="31"/>
+      <c r="AJ3" s="31"/>
+      <c r="AK3" s="33"/>
     </row>
     <row r="4" spans="2:37" ht="9.75" customHeight="1">
-      <c r="B4" s="30"/>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
-      <c r="F4" s="31"/>
-      <c r="G4" s="31"/>
-      <c r="H4" s="31"/>
-      <c r="I4" s="31"/>
-      <c r="J4" s="31"/>
-      <c r="K4" s="31"/>
-      <c r="L4" s="31"/>
-      <c r="M4" s="31"/>
-      <c r="N4" s="31"/>
-      <c r="O4" s="31"/>
-      <c r="P4" s="31"/>
-      <c r="Q4" s="31"/>
-      <c r="R4" s="31"/>
-      <c r="S4" s="31"/>
-      <c r="T4" s="31"/>
-      <c r="U4" s="31"/>
-      <c r="V4" s="31"/>
-      <c r="W4" s="31"/>
-      <c r="X4" s="31"/>
-      <c r="Y4" s="31"/>
-      <c r="Z4" s="31"/>
-      <c r="AA4" s="31"/>
-      <c r="AB4" s="31"/>
-      <c r="AC4" s="31"/>
-      <c r="AD4" s="31"/>
-      <c r="AE4" s="31"/>
-      <c r="AF4" s="31"/>
-      <c r="AG4" s="31"/>
-      <c r="AH4" s="31"/>
-      <c r="AI4" s="31"/>
-      <c r="AJ4" s="31"/>
-      <c r="AK4" s="32"/>
+      <c r="B4" s="34"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="35"/>
+      <c r="G4" s="35"/>
+      <c r="H4" s="35"/>
+      <c r="I4" s="35"/>
+      <c r="J4" s="35"/>
+      <c r="K4" s="35"/>
+      <c r="L4" s="35"/>
+      <c r="M4" s="35"/>
+      <c r="N4" s="35"/>
+      <c r="O4" s="35"/>
+      <c r="P4" s="35"/>
+      <c r="Q4" s="35"/>
+      <c r="R4" s="35"/>
+      <c r="S4" s="35"/>
+      <c r="T4" s="35"/>
+      <c r="U4" s="35"/>
+      <c r="V4" s="35"/>
+      <c r="W4" s="35"/>
+      <c r="X4" s="35"/>
+      <c r="Y4" s="35"/>
+      <c r="Z4" s="35"/>
+      <c r="AA4" s="35"/>
+      <c r="AB4" s="35"/>
+      <c r="AC4" s="35"/>
+      <c r="AD4" s="35"/>
+      <c r="AE4" s="35"/>
+      <c r="AF4" s="35"/>
+      <c r="AG4" s="35"/>
+      <c r="AH4" s="35"/>
+      <c r="AI4" s="35"/>
+      <c r="AJ4" s="35"/>
+      <c r="AK4" s="36"/>
     </row>
     <row r="5" spans="2:37" ht="9.75" customHeight="1">
-      <c r="B5" s="19"/>
+      <c r="B5" s="23"/>
       <c r="C5" s="7"/>
       <c r="D5" s="8"/>
       <c r="E5" s="8"/>
@@ -44676,88 +44681,106 @@
       <c r="AF5" s="9"/>
       <c r="AG5" s="9"/>
       <c r="AH5" s="9"/>
-      <c r="AI5" s="9"/>
-      <c r="AJ5" s="10"/>
-      <c r="AK5" s="11"/>
+      <c r="AI5" s="9">
+        <f>SUM(D5:AH5)</f>
+        <v>0</v>
+      </c>
+      <c r="AJ5" s="17">
+        <f>AL$5*AI5</f>
+        <v>0</v>
+      </c>
+      <c r="AK5" s="17">
+        <f>AM$5*AI5</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="6" spans="2:37" ht="9.75" customHeight="1" thickBot="1">
-      <c r="B6" s="20"/>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="16"/>
-      <c r="H6" s="16"/>
-      <c r="I6" s="16"/>
-      <c r="J6" s="16"/>
-      <c r="K6" s="16"/>
-      <c r="L6" s="16"/>
-      <c r="M6" s="16"/>
-      <c r="N6" s="16"/>
-      <c r="O6" s="16"/>
-      <c r="P6" s="16"/>
-      <c r="Q6" s="16"/>
-      <c r="R6" s="16"/>
-      <c r="S6" s="16"/>
-      <c r="T6" s="16"/>
-      <c r="U6" s="16"/>
-      <c r="V6" s="16"/>
-      <c r="W6" s="17"/>
-      <c r="X6" s="17"/>
-      <c r="Y6" s="17"/>
-      <c r="Z6" s="17"/>
-      <c r="AA6" s="17"/>
-      <c r="AB6" s="17"/>
-      <c r="AC6" s="17"/>
-      <c r="AD6" s="17"/>
-      <c r="AE6" s="17"/>
-      <c r="AF6" s="17"/>
-      <c r="AG6" s="17"/>
-      <c r="AH6" s="17"/>
-      <c r="AI6" s="17"/>
-      <c r="AJ6" s="17"/>
-      <c r="AK6" s="18"/>
+      <c r="B6" s="24"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="11"/>
+      <c r="K6" s="11"/>
+      <c r="L6" s="11"/>
+      <c r="M6" s="11"/>
+      <c r="N6" s="11"/>
+      <c r="O6" s="11"/>
+      <c r="P6" s="11"/>
+      <c r="Q6" s="11"/>
+      <c r="R6" s="11"/>
+      <c r="S6" s="11"/>
+      <c r="T6" s="11"/>
+      <c r="U6" s="11"/>
+      <c r="V6" s="11"/>
+      <c r="W6" s="12"/>
+      <c r="X6" s="12"/>
+      <c r="Y6" s="12"/>
+      <c r="Z6" s="12"/>
+      <c r="AA6" s="12"/>
+      <c r="AB6" s="12"/>
+      <c r="AC6" s="12"/>
+      <c r="AD6" s="12"/>
+      <c r="AE6" s="12"/>
+      <c r="AF6" s="12"/>
+      <c r="AG6" s="12"/>
+      <c r="AH6" s="12"/>
+      <c r="AI6" s="12">
+        <f t="shared" ref="AI6" si="0">SUM(D6:AH6)</f>
+        <v>0</v>
+      </c>
+      <c r="AJ6" s="18">
+        <f>AL$6*AI6</f>
+        <v>0</v>
+      </c>
+      <c r="AK6" s="19">
+        <f>AM$6*AI6</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="2:37" ht="9.75" customHeight="1" thickTop="1">
-      <c r="B7" s="21"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="13"/>
-      <c r="I7" s="13"/>
-      <c r="J7" s="13"/>
-      <c r="K7" s="13"/>
-      <c r="L7" s="13"/>
-      <c r="M7" s="13"/>
-      <c r="N7" s="13"/>
-      <c r="O7" s="13"/>
-      <c r="P7" s="13"/>
-      <c r="Q7" s="13"/>
-      <c r="R7" s="13"/>
-      <c r="S7" s="13"/>
-      <c r="T7" s="13"/>
-      <c r="U7" s="13"/>
-      <c r="V7" s="13"/>
-      <c r="W7" s="13"/>
-      <c r="X7" s="13"/>
-      <c r="Y7" s="13"/>
-      <c r="Z7" s="13"/>
-      <c r="AA7" s="13"/>
-      <c r="AB7" s="13"/>
-      <c r="AC7" s="13"/>
-      <c r="AD7" s="13"/>
-      <c r="AE7" s="13"/>
-      <c r="AF7" s="13"/>
-      <c r="AG7" s="13"/>
-      <c r="AH7" s="13"/>
+      <c r="B7" s="25"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="21"/>
+      <c r="G7" s="21"/>
+      <c r="H7" s="21"/>
+      <c r="I7" s="21"/>
+      <c r="J7" s="21"/>
+      <c r="K7" s="21"/>
+      <c r="L7" s="21"/>
+      <c r="M7" s="21"/>
+      <c r="N7" s="21"/>
+      <c r="O7" s="21"/>
+      <c r="P7" s="21"/>
+      <c r="Q7" s="21"/>
+      <c r="R7" s="21"/>
+      <c r="S7" s="21"/>
+      <c r="T7" s="21"/>
+      <c r="U7" s="21"/>
+      <c r="V7" s="21"/>
+      <c r="W7" s="21"/>
+      <c r="X7" s="21"/>
+      <c r="Y7" s="21"/>
+      <c r="Z7" s="21"/>
+      <c r="AA7" s="21"/>
+      <c r="AB7" s="21"/>
+      <c r="AC7" s="21"/>
+      <c r="AD7" s="21"/>
+      <c r="AE7" s="21"/>
+      <c r="AF7" s="21"/>
+      <c r="AG7" s="21"/>
+      <c r="AH7" s="22"/>
       <c r="AI7" s="13"/>
-      <c r="AJ7" s="13"/>
-      <c r="AK7" s="14"/>
+      <c r="AJ7" s="14"/>
+      <c r="AK7" s="15"/>
     </row>
     <row r="8" spans="2:37" ht="9.75" customHeight="1">
-      <c r="C8" s="15"/>
+      <c r="C8" s="16"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
@@ -44794,7 +44817,7 @@
       <c r="AK8" s="3"/>
     </row>
     <row r="9" spans="2:37" ht="9.75" customHeight="1">
-      <c r="C9" s="15"/>
+      <c r="C9" s="16"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
@@ -44869,21 +44892,20 @@
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="AI2:AI3"/>
     <mergeCell ref="AJ2:AJ3"/>
     <mergeCell ref="AK2:AK3"/>
     <mergeCell ref="B4:AK4"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="AI2:AI3"/>
   </mergeCells>
   <phoneticPr fontId="3"/>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.78374999999999995" bottom="0.39370078740157483" header="0.39370078740157483" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="99" orientation="landscape" r:id="rId1"/>
   <headerFooter>
-    <oddHeader>&amp;L&amp;"MSゴシック,標準"日通システム株式会社
-&amp;C&amp;"MSゴシック,太字"&amp;16月間予約&amp;R&amp;"MSゴシック,標準"&amp;D　&amp;T　
+    <oddHeader>&amp;C&amp;"MSゴシック,太字"&amp;16月間予約台帳&amp;R&amp;"MSゴシック,標準"&amp;D　&amp;T　
 page&amp;P</oddHeader>
   </headerFooter>
   <rowBreaks count="1" manualBreakCount="1">

</xml_diff>